<commit_message>
Added final report and raw data updated to reduce overfitting
</commit_message>
<xml_diff>
--- a/data/processed/processed_data.xlsx
+++ b/data/processed/processed_data.xlsx
@@ -1874,7 +1874,7 @@
         <v>467</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
         <v>468</v>
@@ -1903,7 +1903,7 @@
         <v>467</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>468</v>
@@ -1961,7 +1961,7 @@
         <v>467</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s">
         <v>468</v>
@@ -2048,7 +2048,7 @@
         <v>467</v>
       </c>
       <c r="E9">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
         <v>468</v>
@@ -2077,7 +2077,7 @@
         <v>467</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="s">
         <v>468</v>
@@ -2106,7 +2106,7 @@
         <v>467</v>
       </c>
       <c r="E11">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
         <v>468</v>
@@ -2135,7 +2135,7 @@
         <v>467</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
         <v>468</v>
@@ -2164,7 +2164,7 @@
         <v>467</v>
       </c>
       <c r="E13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
         <v>468</v>
@@ -2216,7 +2216,7 @@
         <v>467</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
         <v>468</v>
@@ -2245,7 +2245,7 @@
         <v>467</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="s">
         <v>469</v>
@@ -2274,7 +2274,7 @@
         <v>467</v>
       </c>
       <c r="E17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="s">
         <v>469</v>
@@ -2303,7 +2303,7 @@
         <v>467</v>
       </c>
       <c r="E18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="s">
         <v>469</v>
@@ -2390,7 +2390,7 @@
         <v>467</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" t="s">
         <v>468</v>
@@ -2448,7 +2448,7 @@
         <v>467</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F23" t="s">
         <v>468</v>
@@ -2477,7 +2477,7 @@
         <v>467</v>
       </c>
       <c r="E24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="s">
         <v>468</v>
@@ -2506,7 +2506,7 @@
         <v>467</v>
       </c>
       <c r="E25">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
         <v>468</v>
@@ -2535,7 +2535,7 @@
         <v>467</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F26" t="s">
         <v>468</v>
@@ -2564,7 +2564,7 @@
         <v>467</v>
       </c>
       <c r="E27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F27" t="s">
         <v>468</v>
@@ -2593,7 +2593,7 @@
         <v>467</v>
       </c>
       <c r="E28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="s">
         <v>469</v>
@@ -2622,7 +2622,7 @@
         <v>467</v>
       </c>
       <c r="E29">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
         <v>469</v>
@@ -2651,7 +2651,7 @@
         <v>467</v>
       </c>
       <c r="E30">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F30" t="s">
         <v>469</v>
@@ -2677,7 +2677,7 @@
         <v>467</v>
       </c>
       <c r="E31">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F31" t="s">
         <v>468</v>
@@ -2764,7 +2764,7 @@
         <v>467</v>
       </c>
       <c r="E34">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F34" t="s">
         <v>468</v>
@@ -2793,7 +2793,7 @@
         <v>467</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F35" t="s">
         <v>468</v>
@@ -2822,7 +2822,7 @@
         <v>467</v>
       </c>
       <c r="E36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F36" t="s">
         <v>468</v>
@@ -2851,7 +2851,7 @@
         <v>467</v>
       </c>
       <c r="E37">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F37" t="s">
         <v>469</v>
@@ -2909,7 +2909,7 @@
         <v>467</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F39" t="s">
         <v>469</v>
@@ -2938,7 +2938,7 @@
         <v>467</v>
       </c>
       <c r="E40">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F40" t="s">
         <v>468</v>
@@ -2967,7 +2967,7 @@
         <v>467</v>
       </c>
       <c r="E41">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F41" t="s">
         <v>468</v>
@@ -3025,7 +3025,7 @@
         <v>467</v>
       </c>
       <c r="E43">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="s">
         <v>468</v>
@@ -3083,7 +3083,7 @@
         <v>467</v>
       </c>
       <c r="E45">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F45" t="s">
         <v>468</v>
@@ -3112,7 +3112,7 @@
         <v>467</v>
       </c>
       <c r="E46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="s">
         <v>468</v>
@@ -3141,7 +3141,7 @@
         <v>467</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F47" t="s">
         <v>468</v>
@@ -3199,7 +3199,7 @@
         <v>467</v>
       </c>
       <c r="E49">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F49" t="s">
         <v>468</v>
@@ -3225,7 +3225,7 @@
         <v>467</v>
       </c>
       <c r="E50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F50" t="s">
         <v>468</v>
@@ -3283,7 +3283,7 @@
         <v>467</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F52" t="s">
         <v>469</v>
@@ -3312,7 +3312,7 @@
         <v>467</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F53" t="s">
         <v>469</v>
@@ -3370,7 +3370,7 @@
         <v>467</v>
       </c>
       <c r="E55">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F55" t="s">
         <v>468</v>
@@ -3399,7 +3399,7 @@
         <v>467</v>
       </c>
       <c r="E56">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F56" t="s">
         <v>468</v>
@@ -3428,7 +3428,7 @@
         <v>467</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F57" t="s">
         <v>468</v>
@@ -3544,7 +3544,7 @@
         <v>467</v>
       </c>
       <c r="E61">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F61" t="s">
         <v>468</v>
@@ -3573,7 +3573,7 @@
         <v>467</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F62" t="s">
         <v>468</v>
@@ -3602,7 +3602,7 @@
         <v>467</v>
       </c>
       <c r="E63">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F63" t="s">
         <v>468</v>
@@ -3631,7 +3631,7 @@
         <v>467</v>
       </c>
       <c r="E64">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F64" t="s">
         <v>468</v>
@@ -3689,7 +3689,7 @@
         <v>467</v>
       </c>
       <c r="E66">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="s">
         <v>468</v>
@@ -3744,7 +3744,7 @@
         <v>467</v>
       </c>
       <c r="E68">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F68" t="s">
         <v>468</v>
@@ -3773,7 +3773,7 @@
         <v>467</v>
       </c>
       <c r="E69">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="s">
         <v>468</v>
@@ -3802,7 +3802,7 @@
         <v>467</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F70" t="s">
         <v>468</v>
@@ -3831,7 +3831,7 @@
         <v>467</v>
       </c>
       <c r="E71">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F71" t="s">
         <v>468</v>
@@ -3889,7 +3889,7 @@
         <v>467</v>
       </c>
       <c r="E73">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="s">
         <v>468</v>
@@ -3918,7 +3918,7 @@
         <v>467</v>
       </c>
       <c r="E74">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F74" t="s">
         <v>468</v>
@@ -3947,7 +3947,7 @@
         <v>467</v>
       </c>
       <c r="E75">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F75" t="s">
         <v>468</v>
@@ -3976,7 +3976,7 @@
         <v>467</v>
       </c>
       <c r="E76">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F76" t="s">
         <v>468</v>
@@ -4005,7 +4005,7 @@
         <v>467</v>
       </c>
       <c r="E77">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F77" t="s">
         <v>468</v>
@@ -4063,7 +4063,7 @@
         <v>467</v>
       </c>
       <c r="E79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F79" t="s">
         <v>468</v>
@@ -4092,7 +4092,7 @@
         <v>467</v>
       </c>
       <c r="E80">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F80" t="s">
         <v>468</v>
@@ -4121,7 +4121,7 @@
         <v>467</v>
       </c>
       <c r="E81">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F81" t="s">
         <v>468</v>
@@ -4150,7 +4150,7 @@
         <v>467</v>
       </c>
       <c r="E82">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F82" t="s">
         <v>468</v>
@@ -4179,7 +4179,7 @@
         <v>467</v>
       </c>
       <c r="E83">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="s">
         <v>468</v>
@@ -4208,7 +4208,7 @@
         <v>467</v>
       </c>
       <c r="E84">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F84" t="s">
         <v>468</v>
@@ -4237,7 +4237,7 @@
         <v>467</v>
       </c>
       <c r="E85">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F85" t="s">
         <v>468</v>
@@ -4266,7 +4266,7 @@
         <v>467</v>
       </c>
       <c r="E86">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F86" t="s">
         <v>468</v>
@@ -4295,7 +4295,7 @@
         <v>467</v>
       </c>
       <c r="E87">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F87" t="s">
         <v>468</v>
@@ -4324,7 +4324,7 @@
         <v>467</v>
       </c>
       <c r="E88">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F88" t="s">
         <v>468</v>
@@ -4353,7 +4353,7 @@
         <v>467</v>
       </c>
       <c r="E89">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F89" t="s">
         <v>468</v>
@@ -4382,7 +4382,7 @@
         <v>467</v>
       </c>
       <c r="E90">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F90" t="s">
         <v>468</v>
@@ -4411,7 +4411,7 @@
         <v>467</v>
       </c>
       <c r="E91">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F91" t="s">
         <v>468</v>
@@ -4440,7 +4440,7 @@
         <v>467</v>
       </c>
       <c r="E92">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F92" t="s">
         <v>468</v>
@@ -4553,7 +4553,7 @@
         <v>467</v>
       </c>
       <c r="E96">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F96" t="s">
         <v>468</v>
@@ -4640,7 +4640,7 @@
         <v>467</v>
       </c>
       <c r="E99">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F99" t="s">
         <v>468</v>
@@ -4669,7 +4669,7 @@
         <v>467</v>
       </c>
       <c r="E100">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F100" t="s">
         <v>468</v>
@@ -4930,7 +4930,7 @@
         <v>467</v>
       </c>
       <c r="E109">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F109" t="s">
         <v>468</v>
@@ -5188,7 +5188,7 @@
         <v>467</v>
       </c>
       <c r="E118">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F118" t="s">
         <v>468</v>
@@ -5275,7 +5275,7 @@
         <v>467</v>
       </c>
       <c r="E121">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F121" t="s">
         <v>468</v>
@@ -5391,7 +5391,7 @@
         <v>467</v>
       </c>
       <c r="E125">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F125" t="s">
         <v>468</v>
@@ -5562,7 +5562,7 @@
         <v>467</v>
       </c>
       <c r="E131">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F131" t="s">
         <v>468</v>
@@ -5591,7 +5591,7 @@
         <v>467</v>
       </c>
       <c r="E132">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F132" t="s">
         <v>468</v>
@@ -5707,7 +5707,7 @@
         <v>467</v>
       </c>
       <c r="E136">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F136" t="s">
         <v>468</v>
@@ -5736,7 +5736,7 @@
         <v>467</v>
       </c>
       <c r="E137">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F137" t="s">
         <v>468</v>
@@ -5765,7 +5765,7 @@
         <v>467</v>
       </c>
       <c r="E138">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F138" t="s">
         <v>468</v>
@@ -5794,7 +5794,7 @@
         <v>467</v>
       </c>
       <c r="E139">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F139" t="s">
         <v>468</v>
@@ -5823,7 +5823,7 @@
         <v>467</v>
       </c>
       <c r="E140">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F140" t="s">
         <v>468</v>
@@ -5907,7 +5907,7 @@
         <v>467</v>
       </c>
       <c r="E143">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F143" t="s">
         <v>468</v>
@@ -6023,7 +6023,7 @@
         <v>467</v>
       </c>
       <c r="E147">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F147" t="s">
         <v>468</v>
@@ -6052,7 +6052,7 @@
         <v>467</v>
       </c>
       <c r="E148">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F148" t="s">
         <v>468</v>
@@ -6197,7 +6197,7 @@
         <v>467</v>
       </c>
       <c r="E153">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F153" t="s">
         <v>468</v>
@@ -6516,7 +6516,7 @@
         <v>467</v>
       </c>
       <c r="E164">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F164" t="s">
         <v>469</v>
@@ -6658,7 +6658,7 @@
         <v>467</v>
       </c>
       <c r="E169">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F169" t="s">
         <v>469</v>
@@ -7238,7 +7238,7 @@
         <v>467</v>
       </c>
       <c r="E189">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F189" t="s">
         <v>468</v>
@@ -7354,7 +7354,7 @@
         <v>467</v>
       </c>
       <c r="E193">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F193" t="s">
         <v>468</v>
@@ -7470,7 +7470,7 @@
         <v>467</v>
       </c>
       <c r="E197">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F197" t="s">
         <v>468</v>
@@ -7528,7 +7528,7 @@
         <v>467</v>
       </c>
       <c r="E199">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F199" t="s">
         <v>468</v>
@@ -7644,7 +7644,7 @@
         <v>467</v>
       </c>
       <c r="E203">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F203" t="s">
         <v>468</v>
@@ -7873,7 +7873,7 @@
         <v>467</v>
       </c>
       <c r="E211">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F211" t="s">
         <v>469</v>
@@ -8076,7 +8076,7 @@
         <v>467</v>
       </c>
       <c r="E218">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F218" t="s">
         <v>468</v>
@@ -8656,7 +8656,7 @@
         <v>467</v>
       </c>
       <c r="E238">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F238" t="s">
         <v>468</v>
@@ -8801,7 +8801,7 @@
         <v>467</v>
       </c>
       <c r="E243">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F243" t="s">
         <v>468</v>
@@ -8830,7 +8830,7 @@
         <v>467</v>
       </c>
       <c r="E244">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F244" t="s">
         <v>468</v>
@@ -8859,7 +8859,7 @@
         <v>467</v>
       </c>
       <c r="E245">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F245" t="s">
         <v>468</v>
@@ -8917,7 +8917,7 @@
         <v>467</v>
       </c>
       <c r="E247">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F247" t="s">
         <v>468</v>
@@ -9378,7 +9378,7 @@
         <v>467</v>
       </c>
       <c r="E263">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F263" t="s">
         <v>468</v>
@@ -9465,7 +9465,7 @@
         <v>467</v>
       </c>
       <c r="E266">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F266" t="s">
         <v>468</v>
@@ -9694,7 +9694,7 @@
         <v>467</v>
       </c>
       <c r="E274">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F274" t="s">
         <v>468</v>
@@ -10213,7 +10213,7 @@
         <v>467</v>
       </c>
       <c r="E292">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F292" t="s">
         <v>468</v>
@@ -10387,7 +10387,7 @@
         <v>467</v>
       </c>
       <c r="E298">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F298" t="s">
         <v>468</v>
@@ -10590,7 +10590,7 @@
         <v>467</v>
       </c>
       <c r="E305">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F305" t="s">
         <v>468</v>
@@ -10703,7 +10703,7 @@
         <v>467</v>
       </c>
       <c r="E309">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F309" t="s">
         <v>468</v>
@@ -10848,7 +10848,7 @@
         <v>467</v>
       </c>
       <c r="E314">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F314" t="s">
         <v>468</v>
@@ -10964,7 +10964,7 @@
         <v>467</v>
       </c>
       <c r="E318">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F318" t="s">
         <v>468</v>
@@ -11196,7 +11196,7 @@
         <v>467</v>
       </c>
       <c r="E326">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F326" t="s">
         <v>468</v>
@@ -11370,7 +11370,7 @@
         <v>467</v>
       </c>
       <c r="E332">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F332" t="s">
         <v>468</v>
@@ -11805,7 +11805,7 @@
         <v>467</v>
       </c>
       <c r="E347">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F347" t="s">
         <v>468</v>
@@ -12124,7 +12124,7 @@
         <v>467</v>
       </c>
       <c r="E358">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F358" t="s">
         <v>468</v>
@@ -12269,7 +12269,7 @@
         <v>467</v>
       </c>
       <c r="E363">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F363" t="s">
         <v>468</v>
@@ -12382,7 +12382,7 @@
         <v>467</v>
       </c>
       <c r="E367">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F367" t="s">
         <v>468</v>
@@ -12469,7 +12469,7 @@
         <v>467</v>
       </c>
       <c r="E370">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F370" t="s">
         <v>468</v>
@@ -12498,7 +12498,7 @@
         <v>467</v>
       </c>
       <c r="E371">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F371" t="s">
         <v>468</v>
@@ -12614,7 +12614,7 @@
         <v>467</v>
       </c>
       <c r="E375">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F375" t="s">
         <v>468</v>
@@ -12759,7 +12759,7 @@
         <v>467</v>
       </c>
       <c r="E380">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F380" t="s">
         <v>469</v>
@@ -12875,7 +12875,7 @@
         <v>467</v>
       </c>
       <c r="E384">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F384" t="s">
         <v>469</v>
@@ -12962,7 +12962,7 @@
         <v>467</v>
       </c>
       <c r="E387">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F387" t="s">
         <v>468</v>
@@ -13049,7 +13049,7 @@
         <v>467</v>
       </c>
       <c r="E390">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F390" t="s">
         <v>469</v>
@@ -13136,7 +13136,7 @@
         <v>467</v>
       </c>
       <c r="E393">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F393" t="s">
         <v>469</v>
@@ -13191,7 +13191,7 @@
         <v>467</v>
       </c>
       <c r="E395">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F395" t="s">
         <v>469</v>
@@ -13278,7 +13278,7 @@
         <v>467</v>
       </c>
       <c r="E398">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F398" t="s">
         <v>468</v>
@@ -13365,7 +13365,7 @@
         <v>467</v>
       </c>
       <c r="E401">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F401" t="s">
         <v>468</v>
@@ -13594,7 +13594,7 @@
         <v>467</v>
       </c>
       <c r="E409">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F409" t="s">
         <v>468</v>
@@ -13652,7 +13652,7 @@
         <v>467</v>
       </c>
       <c r="E411">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F411" t="s">
         <v>468</v>
@@ -13710,7 +13710,7 @@
         <v>467</v>
       </c>
       <c r="E413">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F413" t="s">
         <v>468</v>
@@ -13971,7 +13971,7 @@
         <v>467</v>
       </c>
       <c r="E422">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F422" t="s">
         <v>468</v>
@@ -14029,7 +14029,7 @@
         <v>467</v>
       </c>
       <c r="E424">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F424" t="s">
         <v>468</v>
@@ -14290,7 +14290,7 @@
         <v>467</v>
       </c>
       <c r="E433">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F433" t="s">
         <v>468</v>
@@ -14348,7 +14348,7 @@
         <v>467</v>
       </c>
       <c r="E435">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F435" t="s">
         <v>468</v>
@@ -14464,7 +14464,7 @@
         <v>467</v>
       </c>
       <c r="E439">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F439" t="s">
         <v>468</v>
@@ -14580,7 +14580,7 @@
         <v>467</v>
       </c>
       <c r="E443">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F443" t="s">
         <v>468</v>
@@ -14664,7 +14664,7 @@
         <v>467</v>
       </c>
       <c r="E446">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F446" t="s">
         <v>468</v>
@@ -14722,7 +14722,7 @@
         <v>467</v>
       </c>
       <c r="E448">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F448" t="s">
         <v>468</v>
@@ -14867,7 +14867,7 @@
         <v>467</v>
       </c>
       <c r="E453">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F453" t="s">
         <v>468</v>
@@ -14925,7 +14925,7 @@
         <v>467</v>
       </c>
       <c r="E455">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F455" t="s">
         <v>468</v>
@@ -15012,7 +15012,7 @@
         <v>467</v>
       </c>
       <c r="E458">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F458" t="s">
         <v>468</v>
@@ -15070,7 +15070,7 @@
         <v>467</v>
       </c>
       <c r="E460">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F460" t="s">
         <v>468</v>
@@ -15157,7 +15157,7 @@
         <v>467</v>
       </c>
       <c r="E463">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F463" t="s">
         <v>468</v>
@@ -15302,7 +15302,7 @@
         <v>467</v>
       </c>
       <c r="E468">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F468" t="s">
         <v>468</v>
@@ -15360,7 +15360,7 @@
         <v>467</v>
       </c>
       <c r="E470">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F470" t="s">
         <v>468</v>
@@ -15418,7 +15418,7 @@
         <v>467</v>
       </c>
       <c r="E472">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F472" t="s">
         <v>468</v>
@@ -15476,7 +15476,7 @@
         <v>467</v>
       </c>
       <c r="E474">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F474" t="s">
         <v>468</v>
@@ -15621,7 +15621,7 @@
         <v>467</v>
       </c>
       <c r="E479">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F479" t="s">
         <v>468</v>
@@ -15679,7 +15679,7 @@
         <v>467</v>
       </c>
       <c r="E481">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F481" t="s">
         <v>468</v>
@@ -15908,7 +15908,7 @@
         <v>467</v>
       </c>
       <c r="E489">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F489" t="s">
         <v>468</v>
@@ -16024,7 +16024,7 @@
         <v>467</v>
       </c>
       <c r="E493">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F493" t="s">
         <v>468</v>
@@ -16314,7 +16314,7 @@
         <v>467</v>
       </c>
       <c r="E503">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F503" t="s">
         <v>469</v>
@@ -16398,7 +16398,7 @@
         <v>467</v>
       </c>
       <c r="E506">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F506" t="s">
         <v>469</v>
@@ -16456,7 +16456,7 @@
         <v>467</v>
       </c>
       <c r="E508">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F508" t="s">
         <v>468</v>
@@ -16598,7 +16598,7 @@
         <v>467</v>
       </c>
       <c r="E513">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F513" t="s">
         <v>468</v>
@@ -16627,7 +16627,7 @@
         <v>467</v>
       </c>
       <c r="E514">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F514" t="s">
         <v>468</v>
@@ -16714,7 +16714,7 @@
         <v>467</v>
       </c>
       <c r="E517">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F517" t="s">
         <v>469</v>
@@ -16772,7 +16772,7 @@
         <v>467</v>
       </c>
       <c r="E519">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F519" t="s">
         <v>469</v>
@@ -16830,7 +16830,7 @@
         <v>467</v>
       </c>
       <c r="E521">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F521" t="s">
         <v>469</v>
@@ -16888,7 +16888,7 @@
         <v>467</v>
       </c>
       <c r="E523">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F523" t="s">
         <v>468</v>
@@ -16946,7 +16946,7 @@
         <v>467</v>
       </c>
       <c r="E525">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F525" t="s">
         <v>468</v>
@@ -17004,7 +17004,7 @@
         <v>467</v>
       </c>
       <c r="E527">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F527" t="s">
         <v>468</v>
@@ -17062,7 +17062,7 @@
         <v>467</v>
       </c>
       <c r="E529">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F529" t="s">
         <v>468</v>
@@ -17120,7 +17120,7 @@
         <v>467</v>
       </c>
       <c r="E531">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F531" t="s">
         <v>469</v>
@@ -17265,7 +17265,7 @@
         <v>467</v>
       </c>
       <c r="E536">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F536" t="s">
         <v>468</v>
@@ -17323,7 +17323,7 @@
         <v>467</v>
       </c>
       <c r="E538">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F538" t="s">
         <v>468</v>
@@ -17410,7 +17410,7 @@
         <v>467</v>
       </c>
       <c r="E541">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F541" t="s">
         <v>468</v>
@@ -17468,7 +17468,7 @@
         <v>467</v>
       </c>
       <c r="E543">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F543" t="s">
         <v>468</v>
@@ -17584,7 +17584,7 @@
         <v>467</v>
       </c>
       <c r="E547">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F547" t="s">
         <v>468</v>
@@ -17642,7 +17642,7 @@
         <v>467</v>
       </c>
       <c r="E549">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F549" t="s">
         <v>468</v>
@@ -17700,7 +17700,7 @@
         <v>467</v>
       </c>
       <c r="E551">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F551" t="s">
         <v>468</v>
@@ -17758,7 +17758,7 @@
         <v>467</v>
       </c>
       <c r="E553">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F553" t="s">
         <v>468</v>
@@ -17787,7 +17787,7 @@
         <v>467</v>
       </c>
       <c r="E554">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F554" t="s">
         <v>468</v>
@@ -17903,7 +17903,7 @@
         <v>467</v>
       </c>
       <c r="E558">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F558" t="s">
         <v>468</v>
@@ -17961,7 +17961,7 @@
         <v>467</v>
       </c>
       <c r="E560">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F560" t="s">
         <v>468</v>
@@ -18048,7 +18048,7 @@
         <v>467</v>
       </c>
       <c r="E563">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F563" t="s">
         <v>468</v>
@@ -18106,7 +18106,7 @@
         <v>467</v>
       </c>
       <c r="E565">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F565" t="s">
         <v>468</v>
@@ -18193,7 +18193,7 @@
         <v>467</v>
       </c>
       <c r="E568">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F568" t="s">
         <v>468</v>
@@ -18222,7 +18222,7 @@
         <v>467</v>
       </c>
       <c r="E569">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F569" t="s">
         <v>468</v>
@@ -18338,7 +18338,7 @@
         <v>467</v>
       </c>
       <c r="E573">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F573" t="s">
         <v>468</v>
@@ -18393,7 +18393,7 @@
         <v>467</v>
       </c>
       <c r="E575">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F575" t="s">
         <v>468</v>
@@ -18451,7 +18451,7 @@
         <v>467</v>
       </c>
       <c r="E577">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F577" t="s">
         <v>468</v>
@@ -18538,7 +18538,7 @@
         <v>467</v>
       </c>
       <c r="E580">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F580" t="s">
         <v>468</v>
@@ -18596,7 +18596,7 @@
         <v>467</v>
       </c>
       <c r="E582">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F582" t="s">
         <v>468</v>
@@ -18709,7 +18709,7 @@
         <v>467</v>
       </c>
       <c r="E586">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F586" t="s">
         <v>468</v>
@@ -18825,7 +18825,7 @@
         <v>467</v>
       </c>
       <c r="E590">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F590" t="s">
         <v>468</v>
@@ -18883,7 +18883,7 @@
         <v>467</v>
       </c>
       <c r="E592">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F592" t="s">
         <v>468</v>
@@ -18941,7 +18941,7 @@
         <v>467</v>
       </c>
       <c r="E594">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F594" t="s">
         <v>468</v>
@@ -18999,7 +18999,7 @@
         <v>467</v>
       </c>
       <c r="E596">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F596" t="s">
         <v>469</v>
@@ -19057,7 +19057,7 @@
         <v>467</v>
       </c>
       <c r="E598">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F598" t="s">
         <v>469</v>
@@ -19173,7 +19173,7 @@
         <v>467</v>
       </c>
       <c r="E602">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F602" t="s">
         <v>469</v>
@@ -19434,7 +19434,7 @@
         <v>467</v>
       </c>
       <c r="E611">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F611" t="s">
         <v>469</v>
@@ -19492,7 +19492,7 @@
         <v>467</v>
       </c>
       <c r="E613">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F613" t="s">
         <v>468</v>
@@ -19634,7 +19634,7 @@
         <v>467</v>
       </c>
       <c r="E618">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F618" t="s">
         <v>468</v>
@@ -19692,7 +19692,7 @@
         <v>467</v>
       </c>
       <c r="E620">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F620" t="s">
         <v>468</v>
@@ -19750,7 +19750,7 @@
         <v>467</v>
       </c>
       <c r="E622">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F622" t="s">
         <v>468</v>
@@ -20127,7 +20127,7 @@
         <v>467</v>
       </c>
       <c r="E635">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F635" t="s">
         <v>468</v>
@@ -20214,7 +20214,7 @@
         <v>467</v>
       </c>
       <c r="E638">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F638" t="s">
         <v>468</v>
@@ -20272,7 +20272,7 @@
         <v>467</v>
       </c>
       <c r="E640">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F640" t="s">
         <v>468</v>
@@ -20330,7 +20330,7 @@
         <v>467</v>
       </c>
       <c r="E642">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F642" t="s">
         <v>468</v>
@@ -20388,7 +20388,7 @@
         <v>467</v>
       </c>
       <c r="E644">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F644" t="s">
         <v>468</v>
@@ -20475,7 +20475,7 @@
         <v>467</v>
       </c>
       <c r="E647">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F647" t="s">
         <v>468</v>
@@ -20562,7 +20562,7 @@
         <v>467</v>
       </c>
       <c r="E650">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F650" t="s">
         <v>468</v>
@@ -20736,7 +20736,7 @@
         <v>467</v>
       </c>
       <c r="E656">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F656" t="s">
         <v>469</v>
@@ -20881,7 +20881,7 @@
         <v>467</v>
       </c>
       <c r="E661">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F661" t="s">
         <v>468</v>
@@ -21023,7 +21023,7 @@
         <v>467</v>
       </c>
       <c r="E666">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F666" t="s">
         <v>468</v>
@@ -21139,7 +21139,7 @@
         <v>467</v>
       </c>
       <c r="E670">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F670" t="s">
         <v>469</v>
@@ -21168,7 +21168,7 @@
         <v>467</v>
       </c>
       <c r="E671">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F671" t="s">
         <v>468</v>
@@ -21197,7 +21197,7 @@
         <v>467</v>
       </c>
       <c r="E672">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F672" t="s">
         <v>468</v>
@@ -21226,7 +21226,7 @@
         <v>467</v>
       </c>
       <c r="E673">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F673" t="s">
         <v>468</v>
@@ -21255,7 +21255,7 @@
         <v>467</v>
       </c>
       <c r="E674">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F674" t="s">
         <v>468</v>
@@ -21368,7 +21368,7 @@
         <v>467</v>
       </c>
       <c r="E678">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F678" t="s">
         <v>468</v>
@@ -21426,7 +21426,7 @@
         <v>467</v>
       </c>
       <c r="E680">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F680" t="s">
         <v>468</v>
@@ -21484,7 +21484,7 @@
         <v>467</v>
       </c>
       <c r="E682">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F682" t="s">
         <v>468</v>
@@ -21542,7 +21542,7 @@
         <v>467</v>
       </c>
       <c r="E684">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F684" t="s">
         <v>468</v>
@@ -21600,7 +21600,7 @@
         <v>467</v>
       </c>
       <c r="E686">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F686" t="s">
         <v>468</v>
@@ -21629,7 +21629,7 @@
         <v>467</v>
       </c>
       <c r="E687">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F687" t="s">
         <v>468</v>
@@ -21687,7 +21687,7 @@
         <v>467</v>
       </c>
       <c r="E689">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F689" t="s">
         <v>468</v>
@@ -21716,7 +21716,7 @@
         <v>467</v>
       </c>
       <c r="E690">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F690" t="s">
         <v>468</v>
@@ -21745,7 +21745,7 @@
         <v>467</v>
       </c>
       <c r="E691">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F691" t="s">
         <v>468</v>
@@ -21774,7 +21774,7 @@
         <v>467</v>
       </c>
       <c r="E692">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F692" t="s">
         <v>468</v>
@@ -21800,7 +21800,7 @@
         <v>467</v>
       </c>
       <c r="E693">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F693" t="s">
         <v>468</v>
@@ -21829,7 +21829,7 @@
         <v>467</v>
       </c>
       <c r="E694">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F694" t="s">
         <v>468</v>
@@ -21916,7 +21916,7 @@
         <v>467</v>
       </c>
       <c r="E697">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F697" t="s">
         <v>468</v>
@@ -21974,7 +21974,7 @@
         <v>467</v>
       </c>
       <c r="E699">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F699" t="s">
         <v>468</v>
@@ -22061,7 +22061,7 @@
         <v>467</v>
       </c>
       <c r="E702">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F702" t="s">
         <v>468</v>
@@ -22090,7 +22090,7 @@
         <v>467</v>
       </c>
       <c r="E703">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F703" t="s">
         <v>468</v>
@@ -22177,7 +22177,7 @@
         <v>467</v>
       </c>
       <c r="E706">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F706" t="s">
         <v>468</v>
@@ -22264,7 +22264,7 @@
         <v>467</v>
       </c>
       <c r="E709">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F709" t="s">
         <v>468</v>
@@ -22322,7 +22322,7 @@
         <v>467</v>
       </c>
       <c r="E711">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F711" t="s">
         <v>468</v>
@@ -22409,7 +22409,7 @@
         <v>467</v>
       </c>
       <c r="E714">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F714" t="s">
         <v>468</v>
@@ -22496,7 +22496,7 @@
         <v>467</v>
       </c>
       <c r="E717">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F717" t="s">
         <v>468</v>
@@ -22583,7 +22583,7 @@
         <v>467</v>
       </c>
       <c r="E720">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F720" t="s">
         <v>468</v>
@@ -22728,7 +22728,7 @@
         <v>467</v>
       </c>
       <c r="E725">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F725" t="s">
         <v>469</v>
@@ -22815,7 +22815,7 @@
         <v>467</v>
       </c>
       <c r="E728">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F728" t="s">
         <v>469</v>
@@ -22873,7 +22873,7 @@
         <v>467</v>
       </c>
       <c r="E730">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F730" t="s">
         <v>469</v>
@@ -22902,7 +22902,7 @@
         <v>467</v>
       </c>
       <c r="E731">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F731" t="s">
         <v>469</v>
@@ -23163,7 +23163,7 @@
         <v>467</v>
       </c>
       <c r="E740">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F740" t="s">
         <v>468</v>
@@ -23279,7 +23279,7 @@
         <v>467</v>
       </c>
       <c r="E744">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F744" t="s">
         <v>468</v>
@@ -23366,7 +23366,7 @@
         <v>467</v>
       </c>
       <c r="E747">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F747" t="s">
         <v>469</v>
@@ -23421,7 +23421,7 @@
         <v>467</v>
       </c>
       <c r="E749">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F749" t="s">
         <v>468</v>
@@ -23450,7 +23450,7 @@
         <v>467</v>
       </c>
       <c r="E750">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F750" t="s">
         <v>468</v>
@@ -23537,7 +23537,7 @@
         <v>467</v>
       </c>
       <c r="E753">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F753" t="s">
         <v>468</v>
@@ -23595,7 +23595,7 @@
         <v>467</v>
       </c>
       <c r="E755">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F755" t="s">
         <v>468</v>
@@ -23653,7 +23653,7 @@
         <v>467</v>
       </c>
       <c r="E757">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F757" t="s">
         <v>469</v>
@@ -23740,7 +23740,7 @@
         <v>467</v>
       </c>
       <c r="E760">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F760" t="s">
         <v>468</v>
@@ -23798,7 +23798,7 @@
         <v>467</v>
       </c>
       <c r="E762">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F762" t="s">
         <v>468</v>
@@ -23856,7 +23856,7 @@
         <v>467</v>
       </c>
       <c r="E764">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F764" t="s">
         <v>468</v>
@@ -23914,7 +23914,7 @@
         <v>467</v>
       </c>
       <c r="E766">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F766" t="s">
         <v>468</v>
@@ -23972,7 +23972,7 @@
         <v>467</v>
       </c>
       <c r="E768">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F768" t="s">
         <v>468</v>
@@ -24059,7 +24059,7 @@
         <v>467</v>
       </c>
       <c r="E771">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F771" t="s">
         <v>468</v>
@@ -24117,7 +24117,7 @@
         <v>467</v>
       </c>
       <c r="E773">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F773" t="s">
         <v>468</v>
@@ -24175,7 +24175,7 @@
         <v>467</v>
       </c>
       <c r="E775">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F775" t="s">
         <v>469</v>
@@ -24233,7 +24233,7 @@
         <v>467</v>
       </c>
       <c r="E777">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F777" t="s">
         <v>469</v>
@@ -24291,7 +24291,7 @@
         <v>467</v>
       </c>
       <c r="E779">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F779" t="s">
         <v>468</v>
@@ -24378,7 +24378,7 @@
         <v>467</v>
       </c>
       <c r="E782">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F782" t="s">
         <v>468</v>
@@ -24952,7 +24952,7 @@
         <v>467</v>
       </c>
       <c r="E802">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F802" t="s">
         <v>468</v>
@@ -25039,7 +25039,7 @@
         <v>467</v>
       </c>
       <c r="E805">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F805" t="s">
         <v>468</v>
@@ -25126,7 +25126,7 @@
         <v>467</v>
       </c>
       <c r="E808">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F808" t="s">
         <v>468</v>
@@ -25239,7 +25239,7 @@
         <v>467</v>
       </c>
       <c r="E812">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F812" t="s">
         <v>469</v>
@@ -25297,7 +25297,7 @@
         <v>467</v>
       </c>
       <c r="E814">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F814" t="s">
         <v>469</v>
@@ -25442,7 +25442,7 @@
         <v>467</v>
       </c>
       <c r="E819">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F819" t="s">
         <v>468</v>
@@ -25529,7 +25529,7 @@
         <v>467</v>
       </c>
       <c r="E822">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F822" t="s">
         <v>468</v>
@@ -25587,7 +25587,7 @@
         <v>467</v>
       </c>
       <c r="E824">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F824" t="s">
         <v>468</v>
@@ -25729,7 +25729,7 @@
         <v>467</v>
       </c>
       <c r="E829">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F829" t="s">
         <v>469</v>
@@ -25816,7 +25816,7 @@
         <v>467</v>
       </c>
       <c r="E832">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F832" t="s">
         <v>468</v>
@@ -25990,7 +25990,7 @@
         <v>467</v>
       </c>
       <c r="E838">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F838" t="s">
         <v>469</v>
@@ -26048,7 +26048,7 @@
         <v>467</v>
       </c>
       <c r="E840">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F840" t="s">
         <v>469</v>
@@ -26135,7 +26135,7 @@
         <v>467</v>
       </c>
       <c r="E843">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F843" t="s">
         <v>468</v>
@@ -26216,7 +26216,7 @@
         <v>467</v>
       </c>
       <c r="E846">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F846" t="s">
         <v>468</v>
@@ -26271,7 +26271,7 @@
         <v>467</v>
       </c>
       <c r="E848">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F848" t="s">
         <v>468</v>
@@ -26387,7 +26387,7 @@
         <v>467</v>
       </c>
       <c r="E852">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F852" t="s">
         <v>468</v>
@@ -26474,7 +26474,7 @@
         <v>467</v>
       </c>
       <c r="E855">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F855" t="s">
         <v>469</v>
@@ -26532,7 +26532,7 @@
         <v>467</v>
       </c>
       <c r="E857">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F857" t="s">
         <v>469</v>
@@ -26590,7 +26590,7 @@
         <v>467</v>
       </c>
       <c r="E859">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F859" t="s">
         <v>468</v>
@@ -26648,7 +26648,7 @@
         <v>467</v>
       </c>
       <c r="E861">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F861" t="s">
         <v>468</v>
@@ -26706,7 +26706,7 @@
         <v>467</v>
       </c>
       <c r="E863">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F863" t="s">
         <v>468</v>
@@ -26735,7 +26735,7 @@
         <v>467</v>
       </c>
       <c r="E864">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F864" t="s">
         <v>468</v>
@@ -26764,7 +26764,7 @@
         <v>467</v>
       </c>
       <c r="E865">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F865" t="s">
         <v>468</v>
@@ -26851,7 +26851,7 @@
         <v>467</v>
       </c>
       <c r="E868">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F868" t="s">
         <v>468</v>
@@ -27025,7 +27025,7 @@
         <v>467</v>
       </c>
       <c r="E874">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F874" t="s">
         <v>468</v>
@@ -27112,7 +27112,7 @@
         <v>467</v>
       </c>
       <c r="E877">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F877" t="s">
         <v>468</v>
@@ -27141,7 +27141,7 @@
         <v>467</v>
       </c>
       <c r="E878">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F878" t="s">
         <v>468</v>

</xml_diff>